<commit_message>
Final analysis and results
</commit_message>
<xml_diff>
--- a/tables/ucif_expanded_correct.xlsx
+++ b/tables/ucif_expanded_correct.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>sparsity</t>
+          <t>sparsity_necessary</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>explanation rate</t>
+          <t>necessary explanation rate</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -472,7 +472,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -703,7 +703,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1-best</t>
+          <t>1-delta</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -934,7 +934,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -955,7 +955,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -976,7 +976,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -997,7 +997,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>recent</t>
+          <t>temporal</t>
         </is>
       </c>
     </row>

</xml_diff>